<commit_message>
Additional processing of initial Excel Sheet
</commit_message>
<xml_diff>
--- a/Grocery.xlsx
+++ b/Grocery.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Desktop\DA Class\Kaggle\ML-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A21D35-5E5C-4D1A-9AC0-82A41F500B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9147DE09-1A32-4975-A201-F5F7C654C6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{9EEA7404-9973-453F-9A11-331FBE76B4DB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="95">
   <si>
     <t>Meal Name</t>
   </si>
@@ -95,59 +95,265 @@
     <t>Ingredient 4</t>
   </si>
   <si>
-    <t>Sauce</t>
-  </si>
-  <si>
-    <t>Toppings</t>
-  </si>
-  <si>
-    <t>Crust</t>
-  </si>
-  <si>
     <t>Beef</t>
   </si>
   <si>
     <t>Green Onions</t>
   </si>
   <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>Cheddar</t>
-  </si>
-  <si>
     <t>Ritz</t>
   </si>
   <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>Milk</t>
-  </si>
-  <si>
-    <t>Colby Jack Cheese</t>
-  </si>
-  <si>
-    <t>Fries</t>
-  </si>
-  <si>
-    <t>Buns</t>
-  </si>
-  <si>
     <t>Chicken Stock</t>
   </si>
   <si>
-    <t>Vegetables</t>
+    <t>Baked sweet potatoes, meatballs, fried carrots</t>
+  </si>
+  <si>
+    <t>Chicken wild rice soup with cheese muffins</t>
+  </si>
+  <si>
+    <t>Fried brussel sprouts and gnocchi</t>
+  </si>
+  <si>
+    <t>Mom’s quiche and canned veggie</t>
+  </si>
+  <si>
+    <t>HBH Coq au Vin and mashed potatoes plus asparagus</t>
+  </si>
+  <si>
+    <t>Beef, bean, and corn enchiladas</t>
+  </si>
+  <si>
+    <t>Apple, bacon, cheese panini</t>
+  </si>
+  <si>
+    <t>BBQ pork ribs, mashed potatoes, and broccoli</t>
+  </si>
+  <si>
+    <t>HBH broccoli cheddar chicken and rice casserole</t>
+  </si>
+  <si>
+    <t>Charcuterie board</t>
+  </si>
+  <si>
+    <t>White chicken chili</t>
+  </si>
+  <si>
+    <t>Zucchini and tomato flatbreads</t>
+  </si>
+  <si>
+    <t>Smoothies and egg sammies</t>
+  </si>
+  <si>
+    <t>Pot roast with multi-colored potatoes and carrots</t>
+  </si>
+  <si>
+    <t>Butter chicken wings, mashed potatoes/carrots, and baked beans</t>
+  </si>
+  <si>
+    <t>One sheet sausage, potatoes, broccoli and cauliflower</t>
+  </si>
+  <si>
+    <t>Pumpkin waffles with scrambled eggs and bacon</t>
+  </si>
+  <si>
+    <t>Shepherd's pie and asparagus</t>
+  </si>
+  <si>
+    <t>HBH Spicy sesame noodles with ginger chicken</t>
+  </si>
+  <si>
+    <t>Spaghetti bake and caesar salad</t>
+  </si>
+  <si>
+    <t>Beef stew with all the veg and maybe beer bread</t>
+  </si>
+  <si>
+    <t>HBH One skillet creamy sundried-tomato chicken and orzo</t>
+  </si>
+  <si>
+    <t>Enchilada chicken soup</t>
+  </si>
+  <si>
+    <t>Olive Garden chicken and gnocchi soup</t>
+  </si>
+  <si>
+    <t>One-Pot Swedish meatballs with noodles (Healthy ish board)</t>
+  </si>
+  <si>
+    <t>HBH One Pot 4 Cheese Caprese Mac and Cheese</t>
+  </si>
+  <si>
+    <t>Sweet Potatoes</t>
+  </si>
+  <si>
+    <t>Potatoes</t>
+  </si>
+  <si>
+    <t>Bacon</t>
+  </si>
+  <si>
+    <t>Brussel Sprouts</t>
+  </si>
+  <si>
+    <t>Broccoli</t>
+  </si>
+  <si>
+    <t>Carrots</t>
+  </si>
+  <si>
+    <t>Cheeses</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Baked Beans</t>
+  </si>
+  <si>
+    <t>Ingredient 5</t>
+  </si>
+  <si>
+    <t>Ingredient 6</t>
+  </si>
+  <si>
+    <t>Ingredient 7</t>
+  </si>
+  <si>
+    <t>Ingredient 8</t>
+  </si>
+  <si>
+    <t>Ingredient 9</t>
+  </si>
+  <si>
+    <t>Ingredient 10</t>
+  </si>
+  <si>
+    <t>Lemon</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>Chicken Broth</t>
+  </si>
+  <si>
+    <t>Orzo Pasta</t>
+  </si>
+  <si>
+    <t>Celery</t>
+  </si>
+  <si>
+    <t>Potato Gnocchi</t>
+  </si>
+  <si>
+    <t>Half and half</t>
+  </si>
+  <si>
+    <t>Spinach</t>
+  </si>
+  <si>
+    <t>Rice a Roni Long Grain and Wild Rice</t>
+  </si>
+  <si>
+    <t>scallions</t>
+  </si>
+  <si>
+    <t>Meats</t>
+  </si>
+  <si>
+    <t>Bell Pepper</t>
+  </si>
+  <si>
+    <t>Enchilada Sauce</t>
+  </si>
+  <si>
+    <t>Cream Cheese</t>
+  </si>
+  <si>
+    <t>Diced Tomatoes</t>
+  </si>
+  <si>
+    <t>Black Beans</t>
+  </si>
+  <si>
+    <t>Chicken Breasts</t>
+  </si>
+  <si>
+    <t>Frozen Corn</t>
+  </si>
+  <si>
+    <t>Mozzarella cheese</t>
+  </si>
+  <si>
+    <t>Ingredient 11</t>
+  </si>
+  <si>
+    <t>Cubed Ham</t>
+  </si>
+  <si>
+    <t>Shredded cheese</t>
+  </si>
+  <si>
+    <t>Refried Beans</t>
+  </si>
+  <si>
+    <t>Canned Corn</t>
+  </si>
+  <si>
+    <t>Tortilla Shells</t>
+  </si>
+  <si>
+    <t>Chicken Breast</t>
+  </si>
+  <si>
+    <t>Tomato Paste</t>
+  </si>
+  <si>
+    <t>Cremini mushrooms</t>
+  </si>
+  <si>
+    <t>Dry Red Wine</t>
+  </si>
+  <si>
+    <t>Yukon Gold Potatoes</t>
+  </si>
+  <si>
+    <t>Heavy Cream</t>
+  </si>
+  <si>
+    <t>Parmesan Cheese</t>
+  </si>
+  <si>
+    <t>Gruyere</t>
+  </si>
+  <si>
+    <t>Ingredient 12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,16 +376,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,22 +773,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA1C99A-E869-4BA5-A546-28BA766D18FE}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,84 +812,362 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" t="s">
+        <v>90</v>
+      </c>
+      <c r="K6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
+      <c r="L24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A20" r:id="rId1" xr:uid="{E93970DA-60DC-4456-BFC6-9CA197893CB1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>